<commit_message>
updated feature request list
</commit_message>
<xml_diff>
--- a/EQTool/Files/Feature Ideas.xlsx
+++ b/EQTool/Files/Feature Ideas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\everquest\EqTool\EQTool\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BBA4AE-04CB-46A3-AFB6-E180A3FF5158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB5D329-F306-431B-B2B2-A4FB862AF467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="1545" windowWidth="25800" windowHeight="11850" xr2:uid="{57E9D846-A56C-414B-8195-A6B14CB6F45A}"/>
+    <workbookView xWindow="900" yWindow="1350" windowWidth="25800" windowHeight="11850" xr2:uid="{57E9D846-A56C-414B-8195-A6B14CB6F45A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t>x</t>
   </si>
@@ -199,6 +199,36 @@
   </si>
   <si>
     <t>Summarize spell effects in timer bar description</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>If spell is overwritten (e.g. Gift of Pure Thought overwrites C2), update spell trigger list</t>
+  </si>
+  <si>
+    <t>ewjax</t>
+  </si>
+  <si>
+    <t>Isthan</t>
+  </si>
+  <si>
+    <t>add feature to clear all timers but mine</t>
+  </si>
+  <si>
+    <t>add different coloration for "my damage"</t>
+  </si>
+  <si>
+    <t>Dgc2002</t>
+  </si>
+  <si>
+    <t>Cylance</t>
+  </si>
+  <si>
+    <t>Another Visual and Audio alert for Randoms would be amazing, ideally you can set what will provide a trigger. Eg. 
+1. All (risk is you will get these for others nearby and not in group - but you would be able to turn this off)
+2. /ran 1000 (customizable so that if someone at Angry or Ring 8 roll does roll you can be alerted)
+3. Maybe when a /ran roll is over a value. Eg. if someone does a /ran 1000 and they achieve a number &gt;900 (these sorts of triggers often used in Raid target races etc...</t>
   </si>
 </sst>
 </file>
@@ -263,20 +293,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,339 +638,409 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A870B684-0393-4ED0-80E6-C3F02FAB2480}">
-  <dimension ref="B1:C73"/>
+  <dimension ref="B1:D81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="3.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="163" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="163" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="4" customFormat="1" ht="18.75">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="2:4" s="2" customFormat="1" ht="18.75">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
-      <c r="C3" s="3" t="s">
+    <row r="3" spans="2:4">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.75">
+    <row r="4" spans="2:4" ht="15.75">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.75">
+    <row r="5" spans="2:4" ht="15.75">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.75">
+    <row r="6" spans="2:4" ht="15.75">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.75">
+    <row r="7" spans="2:4" ht="15.75">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
-      <c r="C8" s="5" t="s">
+    <row r="8" spans="2:4">
+      <c r="D8" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="15.75">
+    <row r="9" spans="2:4" ht="15.75">
       <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.75">
+    <row r="10" spans="2:4" ht="15.75">
       <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15.75">
+    <row r="11" spans="2:4" ht="15.75">
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15.75">
+    <row r="12" spans="2:4" ht="15.75">
       <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15.75">
+    <row r="13" spans="2:4" ht="15.75">
       <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="15.75">
+    <row r="14" spans="2:4" ht="15.75">
       <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
-      <c r="C15" s="5" t="s">
+    <row r="15" spans="2:4">
+      <c r="D15" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
-      <c r="C16" s="5" t="s">
+    <row r="16" spans="2:4">
+      <c r="D16" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="3:3">
-      <c r="C17" s="5" t="s">
+    <row r="17" spans="4:4">
+      <c r="D17" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="3:3">
-      <c r="C20" s="3" t="s">
+    <row r="20" spans="4:4">
+      <c r="D20" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="3:3">
-      <c r="C21" t="s">
+    <row r="21" spans="4:4">
+      <c r="D21" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="3:3">
-      <c r="C22" t="s">
+    <row r="22" spans="4:4">
+      <c r="D22" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="3:3">
-      <c r="C23" t="s">
+    <row r="23" spans="4:4">
+      <c r="D23" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="3:3">
-      <c r="C24" t="s">
+    <row r="24" spans="4:4">
+      <c r="D24" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="3:3">
-      <c r="C25" t="s">
+    <row r="25" spans="4:4">
+      <c r="D25" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="3:3">
-      <c r="C26" t="s">
+    <row r="26" spans="4:4">
+      <c r="D26" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="3:3">
-      <c r="C27" t="s">
+    <row r="27" spans="4:4">
+      <c r="D27" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="3:3">
-      <c r="C28" t="s">
+    <row r="28" spans="4:4">
+      <c r="D28" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="3:3">
-      <c r="C29" t="s">
+    <row r="29" spans="4:4">
+      <c r="D29" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="3:3">
-      <c r="C30" t="s">
+    <row r="30" spans="4:4">
+      <c r="D30" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="3:3">
-      <c r="C31" t="s">
+    <row r="31" spans="4:4">
+      <c r="D31" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="3:3">
-      <c r="C32" t="s">
+    <row r="32" spans="4:4">
+      <c r="D32" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="3:3">
-      <c r="C33" t="s">
+    <row r="33" spans="4:4">
+      <c r="D33" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="3:3">
-      <c r="C34" t="s">
+    <row r="34" spans="4:4">
+      <c r="D34" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="3:3">
-      <c r="C35" t="s">
+    <row r="35" spans="4:4">
+      <c r="D35" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="3:3">
-      <c r="C36" t="s">
+    <row r="36" spans="4:4">
+      <c r="D36" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="3:3">
-      <c r="C37" t="s">
+    <row r="37" spans="4:4">
+      <c r="D37" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="3:3">
-      <c r="C38" t="s">
+    <row r="38" spans="4:4">
+      <c r="D38" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="3:3">
-      <c r="C43" s="3" t="s">
+    <row r="43" spans="4:4">
+      <c r="D43" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="3:3">
-      <c r="C44" t="s">
+    <row r="44" spans="4:4">
+      <c r="D44" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="3:3">
-      <c r="C45" t="s">
+    <row r="45" spans="4:4">
+      <c r="D45" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="3:3">
-      <c r="C46" t="s">
+    <row r="46" spans="4:4">
+      <c r="D46" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="3:3">
-      <c r="C47" t="s">
+    <row r="47" spans="4:4">
+      <c r="D47" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="3:3">
-      <c r="C53" s="3" t="s">
+    <row r="53" spans="3:4">
+      <c r="D53" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="3:3">
-      <c r="C54" t="s">
+    <row r="54" spans="3:4">
+      <c r="D54" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="3:3">
-      <c r="C55" t="s">
+    <row r="55" spans="3:4">
+      <c r="D55" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="3:3">
-      <c r="C56" t="s">
+    <row r="56" spans="3:4">
+      <c r="D56" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="3:3">
-      <c r="C59" s="3" t="s">
+    <row r="59" spans="3:4">
+      <c r="D59" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="3:3">
-      <c r="C60" t="s">
+    <row r="60" spans="3:4">
+      <c r="C60" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D60" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="3:3">
-      <c r="C61" t="s">
+    <row r="61" spans="3:4">
+      <c r="C61" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D61" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="3:3">
-      <c r="C62" t="s">
+    <row r="62" spans="3:4">
+      <c r="C62" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D62" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="3:3">
-      <c r="C63" t="s">
+    <row r="63" spans="3:4">
+      <c r="C63" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D63" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="3:3">
-      <c r="C64" t="s">
+    <row r="64" spans="3:4">
+      <c r="C64" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D64" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="3:3">
-      <c r="C65" t="s">
+    <row r="65" spans="3:4">
+      <c r="C65" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D65" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="66" spans="3:3">
-      <c r="C66" t="s">
+    <row r="66" spans="3:4">
+      <c r="C66" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D66" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="3:3">
-      <c r="C69" s="3" t="s">
+    <row r="67" spans="3:4">
+      <c r="C67" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4">
+      <c r="C68" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4">
+      <c r="D71" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="3:3">
-      <c r="C70" t="s">
+    <row r="72" spans="3:4">
+      <c r="C72" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D72" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="3:3">
-      <c r="C71" t="s">
+    <row r="73" spans="3:4">
+      <c r="C73" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D73" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="72" spans="3:3">
-      <c r="C72" t="s">
+    <row r="74" spans="3:4">
+      <c r="C74" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D74" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="3:3">
-      <c r="C73" t="s">
+    <row r="75" spans="3:4">
+      <c r="C75" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D75" s="7" t="s">
         <v>56</v>
       </c>
     </row>
+    <row r="76" spans="3:4">
+      <c r="C76" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="3:4" ht="65.25" customHeight="1">
+      <c r="C77" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="81" ht="15.75" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B1:C1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>

</xml_diff>